<commit_message>
Update of data used
</commit_message>
<xml_diff>
--- a/Data/data2030.xlsx
+++ b/Data/data2030.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="network" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="190">
   <si>
     <t xml:space="preserve">Scénario</t>
   </si>
@@ -55,396 +55,405 @@
     <t xml:space="preserve">generation new</t>
   </si>
   <si>
-    <t xml:space="preserve">['']</t>
+    <t xml:space="preserve">['None']</t>
   </si>
   <si>
     <t xml:space="preserve">production scenario</t>
   </si>
   <si>
+    <t xml:space="preserve">consumption scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vehicles scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buses scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Citalis', 'Karouest', 'Alterneo', 'Carsud', 'Estival']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[49499, 46836, 34567, 20597, 15809]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">climate scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hydrogen 30 bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">darkorange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hydrogen 350 bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">royalblue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ocean thermal energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rosybrown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geothermal energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crimson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bagasse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">darkseagreen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yellowgreen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skyblue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind onshore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind offshore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">steelblue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biogaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">limegreen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">battery charging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aquamarine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">battery discharging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacity factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lifetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">space requirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nominal investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fixed_OM (tot)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fixed_OM (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variable_OM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fuel_cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_max_pu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_min_pu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">committable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start up cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shut down cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min up time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min down time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">up time bf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">down time bf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ramp limit up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ramp limit down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ramp limit on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ramp limit off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min_year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cold start up time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">discount_rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">env_f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">env_v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">water_f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">water_v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_capa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PV+stockage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermique charbon/bagasse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAC bioéthanol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAC fioul/gazole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moteur Diesel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydraulique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bioénergie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eolien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eolien offshore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biomasse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bagasse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geothermie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LE PORT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAINT-PAUL - CIRAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAINT-LEU - CIRAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIGNE-PARADIS - CIRAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LE BARIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROS PITON SAINTE-ROSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GILLOT-AEROPORT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LE COLOSSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Possession</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St Paul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St Leu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le Gol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Langevin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ste Rose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bois Rouge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marquet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tampon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riviere de l'Est</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moufia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St Andre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le Port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le Bras de la Plaine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beaufonds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dattiers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abondance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La Vallee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ste Marie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Takamaka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAC SUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St Pierre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montvert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIERREFONDS-AEROPORT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réseau</t>
+  </si>
+  <si>
     <t xml:space="preserve">80-90</t>
   </si>
   <si>
-    <t xml:space="preserve">consumption scenario</t>
+    <t xml:space="preserve">'100'</t>
   </si>
   <si>
     <t xml:space="preserve">trend</t>
   </si>
   <si>
-    <t xml:space="preserve">vehicles scenario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buses scenario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">actuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">['Citalis', 'Karouest', 'Alterneo', 'Carsud', 'Estival']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[49499, 46836, 34567, 20597, 15809]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">climate scenario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hydrogen 30 bar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">darkorange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hydrogen 350 bar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electricity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">royalblue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">black</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ocean thermal energy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rosybrown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">geothermal energy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">crimson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bagasse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">darkseagreen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yellowgreen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skyblue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">solar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wind onshore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wind offshore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">steelblue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biogaz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">limegreen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">load</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coral</t>
-  </si>
-  <si>
-    <t xml:space="preserve">battery charging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aquamarine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">battery discharging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">technology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">carrier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">capacity factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lifetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">space requirement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nominal investment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fixed_OM (tot)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fixed_OM (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">variable_OM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fuel_cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">efficiency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p_max_pu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p_min_pu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">committable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">start up cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shut down cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min up time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min down time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">up time bf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">down time bf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ramp limit up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ramp limit down</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ramp limit on</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ramp limit off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">max_year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min_year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cold start up time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">discount_rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">env_f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">env_v</t>
-  </si>
-  <si>
-    <t xml:space="preserve">water_f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">water_v</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">False</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PV+stockage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermique charbon/bagasse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAC bioéthanol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAC fioul/gazole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moteur Diesel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hydraulique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bioénergie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eolien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eolien offshore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biomasse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bagasse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geothermie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LE PORT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAINT-PAUL - CIRAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAINT-LEU - CIRAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIGNE-PARADIS - CIRAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LE BARIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GROS PITON SAINTE-ROSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GILLOT-AEROPORT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LE COLOSSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Possession</t>
-  </si>
-  <si>
-    <t xml:space="preserve">St Paul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">St Leu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le Gol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Langevin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ste Rose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bois Rouge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marquet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tampon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Riviere de l'Est</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moufia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">St Andre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le Port</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le Bras de la Plaine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beaufonds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dattiers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abondance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La Vallee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ste Marie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Takamaka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAC SUD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">St Pierre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Montvert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PIERREFONDS-AEROPORT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Réseau</t>
-  </si>
-  <si>
     <t xml:space="preserve">Citalis</t>
   </si>
   <si>
@@ -487,7 +496,7 @@
     <t xml:space="preserve">hydrogen</t>
   </si>
   <si>
-    <t xml:space="preserve">electrolyzer</t>
+    <t xml:space="preserve">electrolyser</t>
   </si>
   <si>
     <t xml:space="preserve">compressor</t>
@@ -500,6 +509,9 @@
   </si>
   <si>
     <t xml:space="preserve">kind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max hours</t>
   </si>
   <si>
     <t xml:space="preserve">efficiency store</t>
@@ -737,7 +749,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -772,6 +784,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -859,7 +875,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -916,8 +932,8 @@
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
+      <c r="B4" s="1" t="n">
+        <v>100</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -927,10 +943,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -940,13 +956,13 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>40</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>212</v>
+        <v>316</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -955,16 +971,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -972,7 +988,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>1</v>
@@ -999,12 +1015,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="S3" activeCellId="0" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1021,203 +1037,289 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.71"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="P1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="0" t="n">
+      <c r="Q1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4" t="n">
         <v>0.9</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="E2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="4" t="n">
         <v>0.6</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="4" t="n">
         <v>0.04</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="J2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" s="0" t="n">
+      <c r="J2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4" t="n">
         <v>3.8</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="4" t="n">
         <f aca="false">956*1000</f>
         <v>956000</v>
       </c>
-      <c r="M2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" s="0" t="s">
+      <c r="M2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="P2" s="0" t="n">
+        <f aca="false">(29.47+0.456)*1000</f>
+        <v>29926</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="n">
         <v>0.9</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0" t="n">
+      <c r="E3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="4" t="n">
         <f aca="false">(1/45)/(1/33)</f>
         <v>0.733333333333333</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="4" t="n">
         <v>0.04</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="J3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="0" t="n">
+      <c r="J3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4" t="n">
         <v>2.8</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3" s="4" t="n">
         <f aca="false">585*1000</f>
         <v>585000</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="4" t="n">
         <f aca="false">0.12*1000</f>
         <v>120</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N3" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="0" t="n">
+      <c r="P3" s="0" t="n">
+        <f aca="false">(244.58+0.537)*1000</f>
+        <v>245117</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <v>0.9</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="0" t="n">
+      <c r="E4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="4" t="n">
         <f aca="false">0.75</f>
         <v>0.75</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="4" t="n">
         <v>0.04</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="J4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="0" t="n">
+      <c r="J4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="L4" s="4" t="n">
         <f aca="false">2400*1000</f>
         <v>2400000</v>
       </c>
-      <c r="M4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="0" t="s">
+      <c r="M4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="0" t="s">
+      <c r="P4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="I5" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="J5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="L5" s="4" t="n">
+        <f aca="false">2400*1000</f>
+        <v>2400000</v>
+      </c>
+      <c r="M5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>90</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1236,221 +1338,233 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.43"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="P1" s="6" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="B2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="n">
         <v>0.985</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="G2" s="4" t="n">
         <v>0.975</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="H2" s="4" t="n">
         <f aca="false">0.1/24/100</f>
         <v>4.16666666666667E-005</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="I2" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="J2" s="4" t="n">
         <v>0.9</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="K2" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="K2" s="0" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" s="0" t="n">
+      <c r="L2" s="4" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="M2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="B3" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="n">
         <v>0.985</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="G3" s="4" t="n">
         <v>0.975</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="H3" s="4" t="n">
         <f aca="false">0.1/24/100</f>
         <v>4.16666666666667E-005</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="I3" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="J3" s="4" t="n">
         <v>0.9</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="K3" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="K3" s="0" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="0" t="n">
+      <c r="L3" s="4" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="M3" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="0" t="n">
+      <c r="B4" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4" t="n">
         <v>0.985</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="G4" s="4" t="n">
         <v>0.975</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="H4" s="4" t="n">
         <f aca="false">0.1/24/100</f>
         <v>4.16666666666667E-005</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="I4" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="J4" s="4" t="n">
         <v>0.9</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="K4" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="K4" s="0" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="0" t="n">
+      <c r="L4" s="4" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="M4" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O4" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1471,10 +1585,10 @@
   </sheetPr>
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="P35" activeCellId="0" sqref="P35"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="W21" activeCellId="0" sqref="W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1495,227 +1609,229 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="U1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="X1" s="6" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="A2" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="n">
         <v>500</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="4" t="n">
         <v>0.985</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="4" t="n">
         <v>0.975</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="4" t="n">
         <f aca="false">0.1/24/100</f>
         <v>4.16666666666667E-005</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="4" t="n">
         <v>0.9</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="4" t="n">
         <v>0.04</v>
       </c>
-      <c r="M2" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <f aca="false">0.622*1000000</f>
-        <v>622000</v>
-      </c>
-      <c r="O2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" s="0" t="n">
+      <c r="M2" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="N2" s="4" t="n">
+        <f aca="false">0.255*1000000</f>
+        <v>255000</v>
+      </c>
+      <c r="O2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" s="4" t="n">
         <v>0.54</v>
       </c>
-      <c r="Q2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" s="0" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="S2" s="0" t="s">
+      <c r="Q2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" s="4" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="S2" s="4" t="s">
         <v>90</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U2" s="0" t="n">
-        <v>0</v>
+        <f aca="false">(227.72+0.988)*1000</f>
+        <v>228708</v>
       </c>
       <c r="V2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="0" t="n">
+      <c r="A3" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="n">
         <v>500</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="0" t="n">
+      <c r="F3" s="4" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4" t="n">
         <v>0.04</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="N3" s="0" t="n">
-        <f aca="false">0.045*1000000</f>
-        <v>45000</v>
-      </c>
-      <c r="O3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="0" t="n">
+      <c r="N3" s="4" t="n">
+        <f aca="false">0.021*1000000</f>
+        <v>21000</v>
+      </c>
+      <c r="O3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="R3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" s="0" t="s">
+      <c r="R3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>20</v>
+      <c r="T3" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="U3" s="0" t="n">
-        <v>0</v>
+        <f aca="false">(8.4925+0.1)*1000</f>
+        <v>8592.5</v>
       </c>
       <c r="V3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="W3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1750,91 +1866,91 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -1855,10 +1971,10 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1869,138 +1985,138 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2024,10 +2140,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="Z1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E27" activeCellId="0" sqref="E27"/>
+      <selection pane="topRight" activeCell="AH14" activeCellId="0" sqref="AH14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2063,105 +2179,108 @@
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>83</v>
       </c>
       <c r="AMG1" s="0"/>
@@ -2171,13 +2290,13 @@
     </row>
     <row r="2" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>84</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>85</v>
@@ -2186,14 +2305,14 @@
         <v>40</v>
       </c>
       <c r="G2" s="7" t="n">
-        <v>4.57</v>
+        <v>4.04</v>
       </c>
       <c r="H2" s="7" t="n">
-        <f aca="false">0.84*1000000</f>
-        <v>840000</v>
+        <f aca="false">0.64*1000000</f>
+        <v>640000</v>
       </c>
       <c r="I2" s="7" t="n">
-        <v>10700</v>
+        <v>8900</v>
       </c>
       <c r="J2" s="7" t="n">
         <v>0</v>
@@ -2241,13 +2360,13 @@
         <v>0</v>
       </c>
       <c r="AF2" s="7" t="n">
-        <v>50</v>
+        <v>43.9</v>
       </c>
       <c r="AG2" s="7" t="n">
         <v>0</v>
       </c>
       <c r="AH2" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AMG2" s="0"/>
       <c r="AMH2" s="0"/>
@@ -2256,17 +2375,20 @@
     </row>
     <row r="3" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>87</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>85</v>
       </c>
+      <c r="H3" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="I3" s="7" t="n">
         <v>0</v>
       </c>
@@ -2316,7 +2438,7 @@
         <v>0</v>
       </c>
       <c r="AF3" s="7" t="n">
-        <v>0</v>
+        <v>43.9</v>
       </c>
       <c r="AG3" s="7" t="n">
         <v>0</v>
@@ -2331,20 +2453,17 @@
     </row>
     <row r="4" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>88</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="I4" s="8" t="n">
-        <v>0</v>
-      </c>
       <c r="J4" s="8" t="n">
         <v>0</v>
       </c>
@@ -2389,9 +2508,6 @@
       </c>
       <c r="Z4" s="8" t="n">
         <v>1</v>
-      </c>
-      <c r="AD4" s="7" t="n">
-        <v>0.04</v>
       </c>
       <c r="AMG4" s="0"/>
       <c r="AMH4" s="0"/>
@@ -2400,13 +2516,13 @@
     </row>
     <row r="5" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>91</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>89</v>
@@ -2418,26 +2534,26 @@
         <v>25</v>
       </c>
       <c r="G5" s="7" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="H5" s="7" t="n">
-        <f aca="false">0.9*1000000</f>
-        <v>900000</v>
+        <f aca="false">0.85*1000000</f>
+        <v>850000</v>
       </c>
       <c r="I5" s="7" t="n">
-        <v>9300</v>
+        <v>8500</v>
       </c>
       <c r="J5" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K5" s="7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L5" s="7" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="7" t="n">
-        <v>0.43</v>
+        <v>0.35</v>
       </c>
       <c r="N5" s="7" t="n">
         <v>0.9</v>
@@ -2479,13 +2595,14 @@
         <v>0</v>
       </c>
       <c r="AF5" s="7" t="n">
-        <v>97.3</v>
+        <v>342.4</v>
       </c>
       <c r="AG5" s="7" t="n">
         <v>0</v>
       </c>
       <c r="AH5" s="7" t="n">
-        <v>0.52</v>
+        <f aca="false">553000/1000</f>
+        <v>553</v>
       </c>
       <c r="AMG5" s="0"/>
       <c r="AMH5" s="0"/>
@@ -2494,20 +2611,17 @@
     </row>
     <row r="6" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>92</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="I6" s="8" t="n">
-        <v>0</v>
-      </c>
       <c r="J6" s="8" t="n">
         <v>0</v>
       </c>
@@ -2552,9 +2666,6 @@
       </c>
       <c r="Z6" s="8" t="n">
         <v>1</v>
-      </c>
-      <c r="AD6" s="7" t="n">
-        <v>0.04</v>
       </c>
       <c r="AMG6" s="0"/>
       <c r="AMH6" s="0"/>
@@ -2563,20 +2674,17 @@
     </row>
     <row r="7" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>93</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="I7" s="8" t="n">
-        <v>0</v>
-      </c>
       <c r="J7" s="8" t="n">
         <v>0</v>
       </c>
@@ -2627,9 +2735,6 @@
       </c>
       <c r="Z7" s="8" t="n">
         <v>0.1</v>
-      </c>
-      <c r="AD7" s="7" t="n">
-        <v>0.04</v>
       </c>
       <c r="AMG7" s="0"/>
       <c r="AMH7" s="0"/>
@@ -2638,13 +2743,13 @@
     </row>
     <row r="8" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>94</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>89</v>
@@ -2655,6 +2760,9 @@
       <c r="F8" s="7" t="n">
         <v>20</v>
       </c>
+      <c r="H8" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="I8" s="7" t="n">
         <v>0</v>
       </c>
@@ -2703,12 +2811,6 @@
       <c r="Z8" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="AA8" s="7" t="n">
-        <v>700000</v>
-      </c>
-      <c r="AB8" s="7" t="n">
-        <v>400000</v>
-      </c>
       <c r="AD8" s="7" t="n">
         <v>0.04</v>
       </c>
@@ -2716,13 +2818,14 @@
         <v>0</v>
       </c>
       <c r="AF8" s="7" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="AG8" s="7" t="n">
         <v>0</v>
       </c>
       <c r="AH8" s="7" t="n">
-        <v>17</v>
+        <f aca="false">208/1000</f>
+        <v>0.208</v>
       </c>
       <c r="AMG8" s="0"/>
       <c r="AMH8" s="0"/>
@@ -2731,13 +2834,13 @@
     </row>
     <row r="9" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>89</v>
@@ -2749,26 +2852,26 @@
         <v>25</v>
       </c>
       <c r="G9" s="7" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="H9" s="7" t="n">
-        <f aca="false">0.9*1000000</f>
-        <v>900000</v>
+        <f aca="false">0.85*1000000</f>
+        <v>850000</v>
       </c>
       <c r="I9" s="7" t="n">
-        <v>9300</v>
+        <v>8500</v>
       </c>
       <c r="J9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="M9" s="7" t="n">
-        <v>0.43</v>
+        <v>0.35</v>
       </c>
       <c r="N9" s="7" t="n">
         <v>0.9</v>
@@ -2810,13 +2913,14 @@
         <v>0</v>
       </c>
       <c r="AF9" s="7" t="n">
-        <v>97.3</v>
+        <v>342.4</v>
       </c>
       <c r="AG9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="AH9" s="7" t="n">
-        <v>24.52</v>
+        <f aca="false">553000/1000</f>
+        <v>553</v>
       </c>
       <c r="AMG9" s="0"/>
       <c r="AMH9" s="0"/>
@@ -2825,13 +2929,13 @@
     </row>
     <row r="10" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>96</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>85</v>
@@ -2840,17 +2944,17 @@
         <v>30</v>
       </c>
       <c r="H10" s="7" t="n">
-        <f aca="false">1.04*1000000</f>
-        <v>1040000</v>
+        <f aca="false">0.96*1000000</f>
+        <v>960000</v>
       </c>
       <c r="I10" s="7" t="n">
-        <v>12600</v>
+        <v>11340</v>
       </c>
       <c r="J10" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K10" s="7" t="n">
-        <v>1.35</v>
+        <v>1.22</v>
       </c>
       <c r="L10" s="7" t="n">
         <v>0</v>
@@ -2892,13 +2996,14 @@
         <v>0</v>
       </c>
       <c r="AF10" s="7" t="n">
-        <v>30</v>
+        <v>14.1</v>
       </c>
       <c r="AG10" s="7" t="n">
         <v>0</v>
       </c>
       <c r="AH10" s="7" t="n">
-        <v>0.5</v>
+        <f aca="false">2020/1000</f>
+        <v>2.02</v>
       </c>
       <c r="AMG10" s="0"/>
       <c r="AMH10" s="0"/>
@@ -2907,13 +3012,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>97</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>85</v>
@@ -2923,20 +3028,20 @@
         <v>30</v>
       </c>
       <c r="G11" s="7" t="n">
-        <v>171.96</v>
+        <v>171.26</v>
       </c>
       <c r="H11" s="7" t="n">
-        <f aca="false">1.8*1000000</f>
-        <v>1800000</v>
+        <f aca="false">1.64*1000000</f>
+        <v>1640000</v>
       </c>
       <c r="I11" s="7" t="n">
-        <v>39000</v>
+        <v>33000</v>
       </c>
       <c r="J11" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K11" s="7" t="n">
-        <v>3.89</v>
+        <v>3.25</v>
       </c>
       <c r="L11" s="7" t="n">
         <v>0</v>
@@ -2944,6 +3049,8 @@
       <c r="M11" s="7" t="n">
         <v>1</v>
       </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
       <c r="P11" s="7" t="s">
         <v>86</v>
       </c>
@@ -2965,6 +3072,8 @@
       <c r="V11" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
       <c r="Y11" s="7" t="n">
         <v>1</v>
       </c>
@@ -2973,6 +3082,7 @@
       </c>
       <c r="AA11" s="7"/>
       <c r="AB11" s="7"/>
+      <c r="AC11" s="4"/>
       <c r="AD11" s="7" t="n">
         <v>0.04</v>
       </c>
@@ -2980,24 +3090,25 @@
         <v>0</v>
       </c>
       <c r="AF11" s="0" t="n">
-        <v>15</v>
+        <v>15.6</v>
       </c>
       <c r="AG11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AH11" s="0" t="n">
-        <v>0.5</v>
+        <f aca="false">130/1000</f>
+        <v>0.13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>98</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>89</v>
@@ -3007,10 +3118,13 @@
         <v>20</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7" t="n">
+        <f aca="false">H9</f>
+        <v>850000</v>
+      </c>
       <c r="I12" s="7" t="n">
         <f aca="false">I9</f>
-        <v>9300</v>
+        <v>8500</v>
       </c>
       <c r="J12" s="7" t="n">
         <v>0</v>
@@ -3052,14 +3166,21 @@
       <c r="V12" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
       <c r="Y12" s="7" t="n">
         <v>1</v>
       </c>
       <c r="Z12" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="AA12" s="7"/>
-      <c r="AB12" s="7"/>
+      <c r="AA12" s="7" t="n">
+        <v>1100000</v>
+      </c>
+      <c r="AB12" s="0" t="n">
+        <v>200000</v>
+      </c>
+      <c r="AC12" s="4"/>
       <c r="AD12" s="7" t="n">
         <v>0.04</v>
       </c>
@@ -3067,24 +3188,28 @@
         <v>0</v>
       </c>
       <c r="AF12" s="0" t="n">
-        <v>97.3</v>
+        <v>228.3</v>
       </c>
       <c r="AG12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AH12" s="0" t="n">
-        <v>24.52</v>
+        <f aca="false">553000/1000</f>
+        <v>553</v>
+      </c>
+      <c r="AI12" s="0" t="n">
+        <v>320.3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>99</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>89</v>
@@ -3094,10 +3219,13 @@
         <v>20</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="H13" s="7" t="n">
+        <f aca="false">H9</f>
+        <v>850000</v>
+      </c>
       <c r="I13" s="7" t="n">
         <f aca="false">I9</f>
-        <v>9300</v>
+        <v>8500</v>
       </c>
       <c r="J13" s="7" t="n">
         <v>0</v>
@@ -3154,6 +3282,7 @@
       </c>
       <c r="AA13" s="7"/>
       <c r="AB13" s="7"/>
+      <c r="AC13" s="4"/>
       <c r="AD13" s="7" t="n">
         <v>0.04</v>
       </c>
@@ -3161,24 +3290,25 @@
         <v>0</v>
       </c>
       <c r="AF13" s="0" t="n">
-        <v>97.3</v>
+        <v>228.3</v>
       </c>
       <c r="AG13" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AH13" s="0" t="n">
-        <v>24.52</v>
+        <f aca="false">553000/1000</f>
+        <v>553</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>100</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>89</v>
@@ -3190,16 +3320,18 @@
         <v>30</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="H14" s="7" t="n">
+        <f aca="false">1.6*1000000</f>
+        <v>1600000</v>
+      </c>
       <c r="I14" s="7" t="n">
         <v>0</v>
       </c>
       <c r="J14" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="K14" s="0" t="n">
-        <f aca="false">0.25*1000</f>
-        <v>250</v>
+      <c r="K14" s="4" t="n">
+        <v>7</v>
       </c>
       <c r="L14" s="7" t="n">
         <v>0</v>
@@ -3234,18 +3366,21 @@
       <c r="V14" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
       <c r="Y14" s="7" t="n">
         <v>1</v>
       </c>
       <c r="Z14" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="AA14" s="0" t="n">
+      <c r="AA14" s="4" t="n">
         <v>60000</v>
       </c>
-      <c r="AB14" s="0" t="n">
+      <c r="AB14" s="4" t="n">
         <v>30000</v>
       </c>
+      <c r="AC14" s="4"/>
       <c r="AD14" s="7" t="n">
         <v>0.04</v>
       </c>
@@ -3253,24 +3388,28 @@
         <v>0</v>
       </c>
       <c r="AF14" s="0" t="n">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="AG14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AH14" s="0" t="n">
-        <v>10</v>
+        <f aca="false">208/1000</f>
+        <v>0.208</v>
+      </c>
+      <c r="AI14" s="0" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>101</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>89</v>
@@ -3285,17 +3424,17 @@
         <v>5</v>
       </c>
       <c r="H15" s="7" t="n">
-        <f aca="false">2.5*1000000</f>
-        <v>2500000</v>
+        <f aca="false">2.38*1000000</f>
+        <v>2380000</v>
       </c>
       <c r="I15" s="7" t="n">
-        <v>21300</v>
+        <v>19900</v>
       </c>
       <c r="J15" s="7" t="n">
         <v>0</v>
       </c>
       <c r="K15" s="7" t="n">
-        <v>6.13</v>
+        <v>5.86</v>
       </c>
       <c r="L15" s="7" t="n">
         <v>0</v>
@@ -3330,19 +3469,21 @@
       <c r="V15" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
       <c r="Y15" s="7" t="n">
         <v>1</v>
       </c>
       <c r="Z15" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="AA15" s="0" t="n">
-        <v>120000</v>
-      </c>
-      <c r="AB15" s="0" t="n">
+      <c r="AA15" s="4" t="n">
+        <v>110000</v>
+      </c>
+      <c r="AB15" s="4" t="n">
         <v>90000</v>
       </c>
-      <c r="AC15" s="0" t="n">
+      <c r="AC15" s="4" t="n">
         <v>2</v>
       </c>
       <c r="AD15" s="7" t="n">
@@ -3352,13 +3493,17 @@
         <v>0</v>
       </c>
       <c r="AF15" s="0" t="n">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="AG15" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AH15" s="0" t="n">
-        <v>10</v>
+        <f aca="false">500000/1000</f>
+        <v>500</v>
+      </c>
+      <c r="AI15" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -3734,7 +3879,7 @@
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3751,19 +3896,19 @@
         <v>136</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="3" t="n">
-        <v>100</v>
+        <v>137</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>117</v>
@@ -3777,7 +3922,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>118</v>
@@ -3791,7 +3936,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>113</v>
@@ -3805,7 +3950,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>114</v>
@@ -3819,7 +3964,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>121</v>
@@ -3865,7 +4010,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3897,7 +4042,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3910,13 +4055,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="3" t="n">
+        <v>137</v>
+      </c>
+      <c r="B1" s="9" t="n">
         <v>100</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
       <c r="D1" s="3"/>
     </row>

</xml_diff>

<commit_message>
Update of model for existing energy batteries
</commit_message>
<xml_diff>
--- a/Data/data2030.xlsx
+++ b/Data/data2030.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="network" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="194">
   <si>
     <t xml:space="preserve">Scénario</t>
   </si>
@@ -517,6 +517,9 @@
     <t xml:space="preserve">kind</t>
   </si>
   <si>
+    <t xml:space="preserve">power</t>
+  </si>
+  <si>
     <t xml:space="preserve">max hours</t>
   </si>
   <si>
@@ -538,7 +541,7 @@
     <t xml:space="preserve">initial state</t>
   </si>
   <si>
-    <t xml:space="preserve">power</t>
+    <t xml:space="preserve">energy</t>
   </si>
   <si>
     <t xml:space="preserve">electrical</t>
@@ -621,7 +624,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -678,12 +681,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -764,7 +761,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -798,10 +795,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1389,18 +1382,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.43"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1414,10 +1407,10 @@
         <v>51</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>162</v>
@@ -1438,21 +1431,24 @@
         <v>167</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1461,7 +1457,7 @@
         <v>124</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>22</v>
@@ -1470,34 +1466,34 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4" t="n">
         <v>0.985</v>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="H2" s="4" t="n">
         <v>0.975</v>
       </c>
-      <c r="H2" s="4" t="n">
+      <c r="I2" s="4" t="n">
         <f aca="false">0.1/24/100</f>
         <v>4.16666666666667E-005</v>
       </c>
-      <c r="I2" s="4" t="n">
+      <c r="J2" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="J2" s="4" t="n">
+      <c r="K2" s="4" t="n">
         <v>0.9</v>
       </c>
-      <c r="K2" s="4" t="n">
+      <c r="L2" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="L2" s="4" t="n">
+      <c r="M2" s="4" t="n">
         <v>1.6</v>
       </c>
-      <c r="M2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="O2" s="0" t="n">
@@ -1507,6 +1503,9 @@
         <v>0</v>
       </c>
       <c r="Q2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1515,7 +1514,7 @@
         <v>113</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>22</v>
@@ -1524,34 +1523,34 @@
         <v>5</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="F3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4" t="n">
         <v>0.985</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="H3" s="4" t="n">
         <v>0.975</v>
       </c>
-      <c r="H3" s="4" t="n">
+      <c r="I3" s="4" t="n">
         <f aca="false">0.1/24/100</f>
         <v>4.16666666666667E-005</v>
       </c>
-      <c r="I3" s="4" t="n">
+      <c r="J3" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="J3" s="4" t="n">
+      <c r="K3" s="4" t="n">
         <v>0.9</v>
       </c>
-      <c r="K3" s="4" t="n">
+      <c r="L3" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="L3" s="4" t="n">
+      <c r="M3" s="4" t="n">
         <v>1.6</v>
       </c>
-      <c r="M3" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="4" t="n">
         <v>0</v>
       </c>
       <c r="O3" s="0" t="n">
@@ -1561,6 +1560,9 @@
         <v>0</v>
       </c>
       <c r="Q3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1569,7 +1571,7 @@
         <v>129</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>22</v>
@@ -1578,34 +1580,34 @@
         <v>5</v>
       </c>
       <c r="E4" s="4" t="n">
+        <v>9.8</v>
+      </c>
+      <c r="F4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="G4" s="4" t="n">
         <v>0.985</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="H4" s="4" t="n">
         <v>0.975</v>
       </c>
-      <c r="H4" s="4" t="n">
+      <c r="I4" s="4" t="n">
         <f aca="false">0.1/24/100</f>
         <v>4.16666666666667E-005</v>
       </c>
-      <c r="I4" s="4" t="n">
+      <c r="J4" s="4" t="n">
         <v>0.1</v>
       </c>
-      <c r="J4" s="4" t="n">
+      <c r="K4" s="4" t="n">
         <v>0.9</v>
       </c>
-      <c r="K4" s="4" t="n">
+      <c r="L4" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="L4" s="4" t="n">
+      <c r="M4" s="4" t="n">
         <v>1.6</v>
       </c>
-      <c r="M4" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="0" t="n">
+      <c r="N4" s="4" t="n">
         <v>0</v>
       </c>
       <c r="O4" s="0" t="n">
@@ -1615,6 +1617,9 @@
         <v>0</v>
       </c>
       <c r="Q4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1675,22 +1680,22 @@
         <v>150</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>79</v>
@@ -1734,13 +1739,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>0</v>
@@ -1811,13 +1816,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>155</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>0</v>
@@ -1917,18 +1922,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1936,37 +1941,37 @@
         <v>149</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1974,34 +1979,34 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2191,7 +2196,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="I20" activeCellId="0" sqref="I20"/>
@@ -3397,7 +3402,7 @@
         <v>30</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="9" t="n">
+      <c r="H14" s="7" t="n">
         <v>8830000</v>
       </c>
       <c r="I14" s="7" t="n">
@@ -4139,7 +4144,7 @@
       <c r="A1" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="10" t="n">
+      <c r="B1" s="9" t="n">
         <v>100</v>
       </c>
       <c r="C1" s="3" t="s">

</xml_diff>